<commit_message>
modified:   C Utilities.lua 	modified:   README.md 	modified:   cheatsheet.xlsx
</commit_message>
<xml_diff>
--- a/cheatsheet.xlsx
+++ b/cheatsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Github\Automation-scripts-for-Aegisub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C413E628-61D1-42AA-8744-2E91EDF365C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA163F4-7F1F-42A4-A719-AA947B4F0DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,6 +30,30 @@
     <author>HP</author>
   </authors>
   <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{8B6D335C-2046-4E32-B0C6-939CFE0F12D3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>HP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+仅供参考</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F2" authorId="0" shapeId="0" xr:uid="{7CBB1151-EBDA-4BC6-8F0F-AC5F25477B01}">
       <text>
         <r>
@@ -39,9 +63,33 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t xml:space="preserve">图片缩放需要imagemagick，
+          <t>图片缩放需要imagemagick，
 也可将1img转化为5img（需要bobo版mod支持）
-</t>
+若不使用该功能则不用担心</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{66F1EDFB-0006-436D-91F7-BF86443536FC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>HP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+AE &gt; crop 依赖imagemagick，不适用该功能可不安装。</t>
         </r>
       </text>
     </comment>
@@ -50,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="133">
   <si>
     <t>Script</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,10 +128,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>«</t>
   </si>
   <si>
@@ -103,23 +147,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>针对mod缩放不支持浮点数精度的解决方案</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>可由bobo版mod替代</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>改变字幕分辨率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>aegisub自带的更改字幕分辨率功能会导致边框与阴影错误</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>imagemagick</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -140,10 +172,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>â</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Jump</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -224,6 +252,401 @@
   </si>
   <si>
     <t>可部分由bobo版mod替代，其不支持图片的旋转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merge Bilangual SUBS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文和英文由\N区分，若无\N则不区分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>pre2_eng/pre1_eng
+next1_eng/next2_eng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pre2_chs/pre1_chs
+next1_chs/next2_chs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将前第二行/前一行/后一行/
+后第二行英文移至本行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将前第二行/前一行/后一行/
+后第二行中文移至本行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fast Tools</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fast_copy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fast_enter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fast_fad_sequence
+(in/out)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fast_clip_iclip
+converter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fast_selection_onward</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选中当前行至最后一行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在逐帧字幕中创建淡入淡出序列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用fad序列而非alpha序列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入\N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拷贝整行字幕
+保留除时间轴外的所有属性</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>相当于Ctrl+V，需先将一整行字幕粘贴至剪贴板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在clip与iclip间切换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Effect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>particle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>粒子效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dissolve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clip_blur/gradient</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>component_split</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拆字效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>柔化clip边缘/
+沿clip边缘创造颜色渐变</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>溶解效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yutils
+xmlsimple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>typewriter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拼音打字机效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xmlsimple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pixelize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>像素化效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text2shape</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将文字转化为形状</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bord_contour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shape2bord</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将形状转化为边框形状</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>边框绘制效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>««</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>template: CD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一种fancy的注释框进出效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Utilities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.7.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AE Sequential Picture
+Importer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Centralize Drawing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(crop)
+imagemagick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导入AE序列图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将矢量绘图的控制点位于图形中心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete Blank Lines(Global)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>aegisub自带的更改字幕分辨率功能
+会导致边框与阴影错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>针对mod缩放不支持浮点数
+精度的解决方案</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete Comment Lines(Global)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除所有空白行
+(包括只有特效标签没有内容的行)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除所有注释行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete SDH Comment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dialog Check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mocha Data Visualization</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没啥用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除SDH内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对白检查器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>包括超长句检查、双语检查
+与时间轴重叠检查</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成Mocha生成行位置等数据的图表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Move!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将特效点放到一个新的位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multiline Importer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Separate Bilingual SUBS by \N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shift Multiline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Swap SUBS Splitted by \N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将多行文字导入到已有的时间轴内</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将中英字幕用\N隔开</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>要求中文在前，英文在后</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将多行字幕内容整体平移
+到前后的时间轴内</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于字幕错位(错行)的简单更正</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将用\N隔开的字幕前后调换位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Replace Plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个带有数学计算功能的匹配替换器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需对LUA PATTERN有一定了解</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XML Analyzer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.4.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>simulator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字幕流量分析(psedo)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>borderadder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slicecutter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timecalculator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字幕过水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字幕肉酱拆分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不同时间格式转换计算器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -231,7 +654,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +686,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -339,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -369,6 +799,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -654,22 +1096,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.05" customHeight="1" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="26.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="33.6640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="56.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="51.44140625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -680,8 +1122,8 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>10</v>
+      <c r="C1" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>2</v>
@@ -696,33 +1138,33 @@
         <v>4</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="5">
+        <v>47</v>
+      </c>
+      <c r="C2" s="12">
         <v>1.2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
@@ -730,219 +1172,869 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1.3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5">
+        <v>47</v>
+      </c>
+      <c r="C4" s="12">
         <v>2.2000000000000002</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>47</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="5">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>22</v>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C7" s="12"/>
       <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C8" s="12"/>
       <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>22</v>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C10" s="12"/>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="1" t="s">
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="B12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="5"/>
+      <c r="G42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="5"/>
+      <c r="G43" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="13"/>
+    </row>
+    <row r="52" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="13"/>
+    </row>
+    <row r="53" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="13"/>
+    </row>
+    <row r="54" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="13"/>
+    </row>
+    <row r="55" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
modified:   README.md 	modified:   cheatsheet.xlsx 	modified:   src/C Merge Bilingual SUBS.lua 	modified:   src/C XML Analyzer.lua
</commit_message>
<xml_diff>
--- a/cheatsheet.xlsx
+++ b/cheatsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Github\Automation-scripts-for-Aegisub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA163F4-7F1F-42A4-A719-AA947B4F0DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FAEF92-3897-45DE-B074-AA923F2B0F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{66F1EDFB-0006-436D-91F7-BF86443536FC}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{66F1EDFB-0006-436D-91F7-BF86443536FC}">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="135">
   <si>
     <t>Script</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -251,19 +251,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>可部分由bobo版mod替代，其不支持图片的旋转</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Merge Bilangual SUBS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>中文和英文由\N区分，若无\N则不区分</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/</t>
   </si>
   <si>
     <t>pre2_eng/pre1_eng
@@ -353,10 +346,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Effect</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -647,6 +636,26 @@
   </si>
   <si>
     <t>不同时间格式转换计算器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大部分可由bobo版mod替代，其不支持图片的旋转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crop功能在BDX修复内存溢出问题后已无需使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>better_bilang_combiner</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个更加智能的双语合并器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1096,10 +1105,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.05" customHeight="1" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1107,8 +1116,8 @@
     <col min="1" max="1" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="33.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.6640625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="33.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="51.44140625" style="1" customWidth="1"/>
@@ -1146,7 +1155,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="12">
         <v>1.2</v>
@@ -1154,17 +1163,14 @@
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
@@ -1172,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3" s="12">
         <v>1.3</v>
@@ -1181,10 +1187,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>7</v>
@@ -1198,7 +1204,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="12">
         <v>2.2000000000000002</v>
@@ -1207,21 +1213,19 @@
         <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>20</v>
@@ -1230,36 +1234,34 @@
         <v>36</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="12">
-        <v>1</v>
+        <v>46</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="5" t="s">
         <v>21</v>
@@ -1268,17 +1270,15 @@
       <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>40</v>
+      <c r="F7" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="4" t="s">
         <v>22</v>
@@ -1287,22 +1287,20 @@
       <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
+      <c r="F8" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>30</v>
@@ -1310,15 +1308,15 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+    <row r="10" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
       <c r="B10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1336,11 +1334,11 @@
         <v>27</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
       <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
@@ -1358,638 +1356,645 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="12">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="4" t="s">
-        <v>41</v>
+      <c r="B13" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="C13" s="12"/>
-      <c r="D13" s="3" t="s">
-        <v>43</v>
+      <c r="D13" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="5" t="s">
-        <v>49</v>
+      <c r="B17" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="1" t="s">
-        <v>57</v>
+      <c r="D18" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>62</v>
-      </c>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
       <c r="B21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="12">
+        <v>51</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="12">
         <v>1.6</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>71</v>
+      <c r="F22" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C24" s="12"/>
-      <c r="D24" s="3" t="s">
-        <v>69</v>
+      <c r="D24" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="5" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>74</v>
+        <v>65</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>71</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>47</v>
+        <v>88</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C35" s="12"/>
-      <c r="D35" s="3" t="s">
-        <v>97</v>
+      <c r="D35" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C36" s="12"/>
-      <c r="D36" s="1" t="s">
-        <v>98</v>
+      <c r="D36" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F39" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G39" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G40" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F41" s="5"/>
+        <v>105</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G41" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
-      <c r="B42" s="4" t="s">
-        <v>110</v>
+      <c r="B42" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>110</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G42" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
       <c r="B43" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F43" s="5"/>
+      <c r="F43" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G43" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C44" s="13"/>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="28.05" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="F46" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C45" s="13" t="s">
+    </row>
+    <row r="47" spans="1:8" ht="28.05" hidden="1" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="B47" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="28.05" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G46" s="2" t="s">
+      <c r="F47" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>17</v>
@@ -1998,23 +2003,34 @@
     <row r="50" spans="1:7" ht="28.05" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="40.799999999999997" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
+      <c r="B51" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="C51" s="13"/>
+      <c r="D51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
@@ -2035,6 +2051,11 @@
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="13"/>
+    </row>
+    <row r="56" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
modified:   .gitignore 	modified:   cheatsheet.xlsx
</commit_message>
<xml_diff>
--- a/cheatsheet.xlsx
+++ b/cheatsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Github\Automation-scripts-for-Aegisub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FAEF92-3897-45DE-B074-AA923F2B0F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB7349A-7737-4917-8696-316A9F57FEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1107,8 +1107,8 @@
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.05" customHeight="1" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2058,6 +2058,7 @@
       <c r="C56" s="13"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="vB0aoMcOZJN8BzIX2fa9TLvveSdq2zwJZfhU/eNJf70n0TGzKUFebxd9vxG8/KnfoN+lxveihI9rPdrLdv0RGg==" saltValue="9LphcrqhIJwB3d/xprN5BA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>